<commit_message>
PROS-7086: sanofi template update
</commit_message>
<xml_diff>
--- a/Projects/SANOFICI/Data/Template.xlsx
+++ b/Projects/SANOFICI/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -852,7 +852,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1021,6 +1021,13 @@
       <charset val="204"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1147,7 +1154,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1344,6 +1351,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="25" fillId="9" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="23" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1356,7 +1367,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1446,14 +1457,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6437246963563"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.080971659919"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.587044534413"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.82995951417"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5465587044534"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3238866396761"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.587044534413"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6882591093117"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0728744939271"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3238866396761"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6882591093117"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2024291497976"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,19 +1722,19 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.82995951417"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="44.4412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.6437246963563"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.3684210526316"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.3684210526316"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="26.4453441295547"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="45.5384615384615"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.7327935222672"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="19.3441295546559"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.7327935222672"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="17.502024291498"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2041,12 +2052,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="25.82995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="24" width="21.914979757085"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="31.9514170040486"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="21.914979757085"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="24" width="17.753036437247"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="26.4453441295547"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="24" width="22.4008097165992"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="24" width="32.8056680161943"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="22.4008097165992"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="24" width="18.1174089068826"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2059,6 +2070,7 @@
         <v>30</v>
       </c>
       <c r="G1" s="16"/>
+      <c r="H1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
@@ -2233,12 +2245,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="31" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="31" width="38.4412955465587"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="31" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="31" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="31" width="15.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="32" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="31" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="31" width="39.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="31" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="31" width="17.502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="31" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="32" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2389,20 +2401,20 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="29.3805668016194"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="36" width="37.2145748987854"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="22.6437246963563"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="27.2995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="26.6882591093117"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="24" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="24" width="18.3684210526316"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="37" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="30.1133603238866"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="36" width="38.1902834008097"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="27.9068825910931"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="24" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="24" width="18.7327935222672"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="37" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2528,21 +2540,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="32.0728744939271"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="44.4412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="19.3441295546559"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="18.1174089068826"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="27.0566801619433"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="44" width="18.3684210526316"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="45" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="32.9271255060729"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="45.5384615384615"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="19.82995951417"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="18.4898785425101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="27.663967611336"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="44" width="18.7327935222672"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="45" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2737,8 +2749,8 @@
       <c r="E9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="47" t="n">
-        <v>2</v>
+      <c r="F9" s="49" t="n">
+        <v>1</v>
       </c>
       <c r="G9" s="47" t="n">
         <v>1</v>
@@ -2836,20 +2848,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="49" t="s">
+    <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="51" t="n">
+      <c r="C14" s="52" t="n">
         <v>3582910075820</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="53" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="47" t="n">
@@ -2859,34 +2871,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="49" t="s">
+    <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="51" t="n">
+      <c r="C15" s="52" t="n">
         <v>3582910075813</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="47" t="n">
-        <v>4</v>
-      </c>
-      <c r="G15" s="47" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="49" t="s">
+      <c r="F15" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="49" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="51" t="s">
         <v>73</v>
       </c>
       <c r="C16" s="21" t="n">
@@ -2905,11 +2917,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="49" t="s">
+    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="51" t="s">
         <v>74</v>
       </c>
       <c r="C17" s="21" t="n">
@@ -2918,7 +2930,7 @@
       <c r="D17" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="53" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="47" t="n">
@@ -2928,11 +2940,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="49" t="s">
+    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="51" t="s">
         <v>75</v>
       </c>
       <c r="C18" s="21" t="n">
@@ -2951,11 +2963,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="49" t="s">
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="51" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="21" t="n">
@@ -2967,13 +2979,14 @@
       <c r="E19" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="47" t="n">
-        <v>4</v>
-      </c>
-      <c r="G19" s="47" t="n">
-        <v>4</v>
-      </c>
-    </row>
+      <c r="F19" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="G19" s="49" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>

</xml_diff>